<commit_message>
Skill - Barbarian - War Cry: - Damage increased by about 30% - War Cry's mana cost now increases by only 0.75 per level instead of 1
</commit_message>
<xml_diff>
--- a/Global/Excel/Skills.xlsx
+++ b/Global/Excel/Skills.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AA572229-47FA-4DBE-9FA4-CD313221FB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4090DD36-4DD0-404C-B363-70410BCAECAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15329" uniqueCount="2669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15329" uniqueCount="2678">
   <si>
     <t>skill</t>
   </si>
@@ -8027,12 +8027,48 @@
   </si>
   <si>
     <t>siegebeast_attack_1</t>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>40</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>12</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>14</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8980,14 +9016,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="HG112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="HY156" sqref="HY156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -32954,13 +32990,13 @@
         <v>259</v>
       </c>
       <c r="FR156" s="1" t="s">
-        <v>264</v>
+        <v>2669</v>
       </c>
       <c r="FS156" s="1" t="s">
-        <v>298</v>
+        <v>2670</v>
       </c>
       <c r="FT156" s="1" t="s">
-        <v>259</v>
+        <v>2671</v>
       </c>
       <c r="FU156" s="1" t="s">
         <v>259</v>
@@ -32990,40 +33026,40 @@
         <v>264</v>
       </c>
       <c r="HM156" s="1" t="s">
-        <v>295</v>
+        <v>2672</v>
       </c>
       <c r="HN156" s="1" t="s">
-        <v>290</v>
+        <v>2673</v>
       </c>
       <c r="HO156" s="1" t="s">
-        <v>303</v>
+        <v>2674</v>
       </c>
       <c r="HP156" s="1" t="s">
-        <v>264</v>
+        <v>2675</v>
       </c>
       <c r="HQ156" s="1" t="s">
-        <v>299</v>
+        <v>2676</v>
       </c>
       <c r="HR156" s="1" t="s">
-        <v>298</v>
+        <v>2677</v>
       </c>
       <c r="HS156" s="1" t="s">
-        <v>365</v>
+        <v>2670</v>
       </c>
       <c r="HT156" s="1" t="s">
-        <v>290</v>
+        <v>2673</v>
       </c>
       <c r="HU156" s="1" t="s">
-        <v>303</v>
+        <v>2674</v>
       </c>
       <c r="HV156" s="1" t="s">
-        <v>264</v>
+        <v>2675</v>
       </c>
       <c r="HW156" s="1" t="s">
-        <v>299</v>
+        <v>2676</v>
       </c>
       <c r="HX156" s="1" t="s">
-        <v>298</v>
+        <v>2677</v>
       </c>
       <c r="HY156" s="1" t="s">
         <v>1618</v>

</xml_diff>

<commit_message>
Skill - Barbarian - Shout: - Duration baseline increased from 20 seconds to 30 seconds (matching Battle Orders)
</commit_message>
<xml_diff>
--- a/Global/Excel/Skills.xlsx
+++ b/Global/Excel/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4090DD36-4DD0-404C-B363-70410BCAECAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DA805B-8035-4040-B909-F42B7B8C8F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15329" uniqueCount="2678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15329" uniqueCount="2679">
   <si>
     <t>skill</t>
   </si>
@@ -8062,6 +8062,10 @@
   </si>
   <si>
     <t>14</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>750</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9020,10 +9024,10 @@
   <dimension ref="A1:IV359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="HG112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="GL112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="HY156" sqref="HY156"/>
+      <selection pane="bottomRight" activeCell="GQ140" sqref="GQ140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -30771,7 +30775,7 @@
         <v>845</v>
       </c>
       <c r="GQ140" s="1" t="s">
-        <v>722</v>
+        <v>2678</v>
       </c>
       <c r="GR140" s="1" t="s">
         <v>329</v>

</xml_diff>

<commit_message>
Skill - Paladin - Holy Fire: - Damage scales based on distance to the caster. Aura will deal double damage at melee range and linearly scale to normal damage at maximum range (may not work in 1.13) - Resist Fire Synergy increased from 18 to 21% - Damage level scaling increased to 70% - Salvation synergy increased from 6% to 10%
</commit_message>
<xml_diff>
--- a/Global/Excel/Skills.xlsx
+++ b/Global/Excel/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFD4B76-D518-4301-B705-696492AB3148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55743569-56B3-4AB5-9B5E-09D8A99E7884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15374" uniqueCount="2707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15376" uniqueCount="2713">
   <si>
     <t>skill</t>
   </si>
@@ -8167,6 +8167,29 @@
   </si>
   <si>
     <t>par7+skill('Increased Stamina'.blvl)*10</t>
+  </si>
+  <si>
+    <t>Area Damage % Range Scaling (from 100% to 100+X% damage, based on how close the enemy position is to the caster)</t>
+  </si>
+  <si>
+    <t>21</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -9124,10 +9147,10 @@
   <dimension ref="A1:IV359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="HH149" sqref="HH149"/>
+      <selection pane="bottomRight" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -25465,14 +25488,20 @@
       <c r="GV104" s="1" t="s">
         <v>1209</v>
       </c>
+      <c r="GW104" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="GX104" s="1" t="s">
+        <v>2707</v>
+      </c>
       <c r="GY104" s="1" t="s">
-        <v>290</v>
+        <v>2670</v>
       </c>
       <c r="GZ104" s="1" t="s">
         <v>308</v>
       </c>
       <c r="HA104" s="1" t="s">
-        <v>395</v>
+        <v>2708</v>
       </c>
       <c r="HB104" s="1" t="s">
         <v>308</v>
@@ -25496,34 +25525,34 @@
         <v>259</v>
       </c>
       <c r="IC104" s="1" t="s">
-        <v>267</v>
+        <v>2709</v>
       </c>
       <c r="ID104" s="1" t="s">
-        <v>275</v>
+        <v>2664</v>
       </c>
       <c r="IE104" s="1" t="s">
-        <v>284</v>
+        <v>2710</v>
       </c>
       <c r="IF104" s="1" t="s">
-        <v>303</v>
+        <v>2668</v>
       </c>
       <c r="IG104" s="1" t="s">
         <v>290</v>
       </c>
       <c r="IH104" s="1" t="s">
-        <v>259</v>
+        <v>2711</v>
       </c>
       <c r="II104" s="1" t="s">
-        <v>267</v>
+        <v>2712</v>
       </c>
       <c r="IJ104" s="1" t="s">
-        <v>275</v>
+        <v>2710</v>
       </c>
       <c r="IK104" s="1" t="s">
-        <v>284</v>
+        <v>2668</v>
       </c>
       <c r="IL104" s="1" t="s">
-        <v>303</v>
+        <v>2669</v>
       </c>
       <c r="IM104" s="1" t="s">
         <v>1210</v>

</xml_diff>

<commit_message>
Skill - Paladin - Holy Freeze: - Damage scales based on distance to the caster. Aura will deal double damage at melee range and linearly scale to normal damage at maximum range (may not work in 1.13)
Skill - Paladin - Holy Shock
- Damage scales based on distance to the caster. Aura will deal double damage at melee range and linearly scale to normal damage at maximum range (may not work in 1.13)

Skill - Paladin - Sanctuary
Damage scales based on distance to the caster. Aura will deal double damage at melee range and linearly scale to normal damage at maximum range (may not work in 1.13)

Skill - Paladin - Thorns
- Now deals a flat amount of damage when attacked in addition to returning a percentage of damage taken to the enemy when hit
</commit_message>
<xml_diff>
--- a/Global/Excel/Skills.xlsx
+++ b/Global/Excel/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55743569-56B3-4AB5-9B5E-09D8A99E7884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B57366-4CB8-4C4A-A45F-C81B8C249A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15376" uniqueCount="2713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15386" uniqueCount="2714">
   <si>
     <t>skill</t>
   </si>
@@ -8189,6 +8189,10 @@
   </si>
   <si>
     <t>5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ln34</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -9147,10 +9151,10 @@
   <dimension ref="A1:IV359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="HY81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B104" sqref="B104"/>
+      <selection pane="bottomRight" activeCell="IB105" sqref="IB105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -25596,7 +25600,13 @@
         <v>1092</v>
       </c>
       <c r="AB105" s="1" t="s">
-        <v>317</v>
+        <v>1123</v>
+      </c>
+      <c r="AC105" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AD105" s="1" t="s">
+        <v>2713</v>
       </c>
       <c r="DF105" s="1" t="s">
         <v>259</v>
@@ -25669,6 +25679,24 @@
       </c>
       <c r="HK105" s="1" t="s">
         <v>264</v>
+      </c>
+      <c r="IA105" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="IB105" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="IC105" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="ID105" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="IE105" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="IF105" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="IU105" s="1" t="s">
         <v>366</v>
@@ -27325,10 +27353,10 @@
         <v>1209</v>
       </c>
       <c r="GW116" s="1" t="s">
-        <v>257</v>
+        <v>330</v>
       </c>
       <c r="GX116" s="1" t="s">
-        <v>1220</v>
+        <v>2707</v>
       </c>
       <c r="GY116" s="1" t="s">
         <v>303</v>
@@ -27981,10 +28009,10 @@
         <v>1209</v>
       </c>
       <c r="GW120" s="1" t="s">
-        <v>257</v>
+        <v>330</v>
       </c>
       <c r="GX120" s="1" t="s">
-        <v>1220</v>
+        <v>2707</v>
       </c>
       <c r="GY120" s="1" t="s">
         <v>269</v>
@@ -28176,6 +28204,12 @@
       </c>
       <c r="GX121" s="1" t="s">
         <v>1356</v>
+      </c>
+      <c r="GY121" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="GZ121" s="1" t="s">
+        <v>2707</v>
       </c>
       <c r="HA121" s="1" t="s">
         <v>303</v>

</xml_diff>

<commit_message>
Skill - Paladin - Fist of the Heavens: - Now damages Demons in addition to Undead - Casting Delay reduced from 1 second to 0.4 seconds - Holy Bolts now pierce targets
</commit_message>
<xml_diff>
--- a/Global/Excel/Skills.xlsx
+++ b/Global/Excel/Skills.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Games\Diablo II LOD\data\Global\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AD1D8C-9B58-4780-A2AF-73B6E38BF27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D090CE23-366E-44C7-B648-AB7F283DCB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9170,10 +9170,10 @@
   <dimension ref="A1:IV359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="GL80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="ET80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="GS118" sqref="GS118"/>
+      <selection pane="bottomRight" activeCell="FJ123" sqref="FJ123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -28538,7 +28538,7 @@
         <v>1314</v>
       </c>
       <c r="FJ123" s="1" t="s">
-        <v>326</v>
+        <v>2669</v>
       </c>
       <c r="FK123" s="1" t="s">
         <v>259</v>

</xml_diff>